<commit_message>
Agregando P4 y P5
</commit_message>
<xml_diff>
--- a/P4/Cuestionario SUS DIU.xlsx
+++ b/P4/Cuestionario SUS DIU.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="612" yWindow="516" windowWidth="21852" windowHeight="8940"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>EQUIPO:                                           (fecha)</t>
   </si>
@@ -77,17 +80,22 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">Valoracion </t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>User1</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t xml:space="preserve">  (entre 1-5)</t>
     </r>
   </si>
@@ -96,49 +104,64 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">Valoracion </t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>User2</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t xml:space="preserve">  (entre 1-5)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">Valoracion </t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>User3</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t xml:space="preserve">  (entre 1-5)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">Valoracion </t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>User3</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t xml:space="preserve">  (entre 1-5)</t>
     </r>
   </si>
@@ -183,65 +206,85 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">MARGINAL </t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>D</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t xml:space="preserve"> (ENTRE 60-70)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
       <t>ACEPTABLE TIPO</t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> C </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t>(GOOD 70-80)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">ACEPTABLE TIPO </t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">B </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t>(EXECELENT 70-80)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">ACEPTABLE TIPO </t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">A </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t>(THE BEST 90-100)</t>
     </r>
   </si>
@@ -250,37 +293,88 @@
   </si>
   <si>
     <t>http://www.measuringux.com/sus/SUS.pdf</t>
+  </si>
+  <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>Funcionario</t>
+  </si>
+  <si>
+    <t>Intermedio</t>
+  </si>
+  <si>
+    <t>El usuario 1 es un padre de familia de mediana edad que trabaja de funcionario. Le gusta mucho estudiar idiomas y se encuentra algo triste</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>El usuario 4 es una mujer descapacitada bastante planificadora y tiene algo de miedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mujer </t>
+  </si>
+  <si>
+    <t>Estudiante</t>
+  </si>
+  <si>
+    <t>Avanzado</t>
+  </si>
+  <si>
+    <t>Estudiante con una discapacidad de movilidad que se encuentra disgustada</t>
+  </si>
+  <si>
+    <t>Becario</t>
+  </si>
+  <si>
+    <t>El usuario 3 es una persona sociable, interesado en aprender idiomas y está sorprendido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="7">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <b/>
-    </font>
-    <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -288,7 +382,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -304,38 +398,52 @@
     </fill>
   </fills>
   <borders count="17">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thick">
         <color rgb="FF0000FF"/>
       </left>
+      <right/>
       <top style="thick">
         <color rgb="FF0000FF"/>
       </top>
       <bottom style="thick">
         <color rgb="FF0000FF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thick">
         <color rgb="FF0000FF"/>
       </top>
       <bottom style="thick">
         <color rgb="FF0000FF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
         <color rgb="FF00FF00"/>
       </left>
+      <right/>
       <top style="thick">
         <color rgb="FF00FF00"/>
       </top>
       <bottom style="thick">
         <color rgb="FF00FF00"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thick">
         <color rgb="FF00FF00"/>
       </right>
@@ -345,21 +453,34 @@
       <bottom style="thick">
         <color rgb="FF00FF00"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
         <color rgb="FF0000FF"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thick">
         <color rgb="FF00FF00"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
         <color rgb="FF00FF00"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -374,17 +495,20 @@
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FFCCCCCC"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FFCCCCCC"/>
       </top>
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -399,6 +523,7 @@
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -413,6 +538,7 @@
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -427,206 +553,497 @@
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
         <color rgb="FF0000FF"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thick">
         <color rgb="FF0000FF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thick">
         <color rgb="FF0000FF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
         <color rgb="FF00FF00"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thick">
         <color rgb="FF00FF00"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thick">
         <color rgb="FF00FF00"/>
       </right>
+      <top/>
       <bottom style="thick">
         <color rgb="FF00FF00"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="48">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="13" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="14" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="15" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="16" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:K1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.29"/>
-    <col customWidth="1" min="2" max="2" width="50.71"/>
-    <col customWidth="1" min="3" max="3" width="27.86"/>
-    <col customWidth="1" hidden="1" min="4" max="4" width="27.86"/>
-    <col customWidth="1" min="5" max="7" width="27.86"/>
-    <col customWidth="1" min="8" max="8" width="22.0"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="7" width="27.88671875" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:11" ht="16.5" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +1054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -649,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -664,11 +1081,11 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" ht="15.0" customHeight="1">
+    <row r="4" spans="1:11" ht="15" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="44" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="9"/>
@@ -682,64 +1099,104 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" ht="15.0" customHeight="1">
+    <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="44" t="s">
+        <v>45</v>
+      </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" ht="15.0" customHeight="1">
+      <c r="E5" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12">
+        <v>46</v>
+      </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" ht="15.0" customHeight="1">
+      <c r="E6" s="10">
+        <v>23</v>
+      </c>
+      <c r="F6" s="13">
+        <v>28</v>
+      </c>
+      <c r="G6" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="44" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" ht="15.0" customHeight="1">
+      <c r="E7" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="44" t="s">
+        <v>47</v>
+      </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" ht="15.0" customHeight="1">
+      <c r="E8" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" ht="9.75" customHeight="1">
+      <c r="E9" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="9.75" customHeight="1">
       <c r="B10" s="7"/>
       <c r="C10" s="14"/>
       <c r="E10" s="15"/>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="C11" s="14" t="s">
         <v>18</v>
       </c>
@@ -753,7 +1210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:11" ht="14.25" customHeight="1">
       <c r="C12" s="14" t="s">
         <v>19</v>
       </c>
@@ -772,7 +1229,7 @@
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="19" t="s">
         <v>20</v>
@@ -797,294 +1254,374 @@
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
     </row>
-    <row r="14" ht="25.5" customHeight="1">
+    <row r="14" spans="1:11" ht="25.5" customHeight="1">
       <c r="A14" s="25">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="27"/>
+      <c r="C14" s="27">
+        <v>1</v>
+      </c>
       <c r="D14" s="28">
         <f>C14-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="29">
+        <v>1</v>
+      </c>
+      <c r="F14" s="30">
+        <v>1</v>
+      </c>
+      <c r="G14" s="31">
+        <v>1</v>
+      </c>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
     </row>
-    <row r="15" ht="25.5" customHeight="1">
+    <row r="15" spans="1:11" ht="25.5" customHeight="1">
       <c r="A15" s="25">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="27">
+        <v>2</v>
+      </c>
       <c r="D15" s="28">
         <f>5-C15</f>
-        <v>5</v>
-      </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+        <v>3</v>
+      </c>
+      <c r="E15" s="29">
+        <v>2</v>
+      </c>
+      <c r="F15" s="32">
+        <v>1</v>
+      </c>
+      <c r="G15" s="33">
+        <v>3</v>
+      </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" ht="25.5" customHeight="1">
+    <row r="16" spans="1:11" ht="25.5" customHeight="1">
       <c r="A16" s="25">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="27">
+        <v>5</v>
+      </c>
       <c r="D16" s="28">
         <f>C16-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
+        <v>4</v>
+      </c>
+      <c r="E16" s="29">
+        <v>4</v>
+      </c>
+      <c r="F16" s="32">
+        <v>5</v>
+      </c>
+      <c r="G16" s="33">
+        <v>3</v>
+      </c>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
     </row>
-    <row r="17" ht="25.5" customHeight="1">
+    <row r="17" spans="1:11" ht="25.5" customHeight="1">
       <c r="A17" s="25">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="27">
+        <v>1</v>
+      </c>
       <c r="D17" s="28">
         <f>5-C17</f>
-        <v>5</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="32">
+        <v>1</v>
+      </c>
+      <c r="G17" s="33">
+        <v>1</v>
+      </c>
       <c r="H17" s="34"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
     </row>
-    <row r="18" ht="25.5" customHeight="1">
+    <row r="18" spans="1:11" ht="25.5" customHeight="1">
       <c r="A18" s="25">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="27"/>
+      <c r="C18" s="27">
+        <v>4</v>
+      </c>
       <c r="D18" s="28">
         <f>C18-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
+        <v>3</v>
+      </c>
+      <c r="E18" s="29">
+        <v>5</v>
+      </c>
+      <c r="F18" s="32">
+        <v>5</v>
+      </c>
+      <c r="G18" s="33">
+        <v>4</v>
+      </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" ht="25.5" customHeight="1">
+    <row r="19" spans="1:11" ht="25.5" customHeight="1">
       <c r="A19" s="25">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="27">
+        <v>2</v>
+      </c>
       <c r="D19" s="28">
         <f>5-C19</f>
-        <v>5</v>
-      </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
+        <v>3</v>
+      </c>
+      <c r="E19" s="29">
+        <v>2</v>
+      </c>
+      <c r="F19" s="32">
+        <v>1</v>
+      </c>
+      <c r="G19" s="33">
+        <v>1</v>
+      </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" ht="25.5" customHeight="1">
+    <row r="20" spans="1:11" ht="25.5" customHeight="1">
       <c r="A20" s="25">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="27"/>
+      <c r="C20" s="27">
+        <v>4</v>
+      </c>
       <c r="D20" s="28">
         <f>C20-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+        <v>3</v>
+      </c>
+      <c r="E20" s="29">
+        <v>4</v>
+      </c>
+      <c r="F20" s="32">
+        <v>4</v>
+      </c>
+      <c r="G20" s="33">
+        <v>4</v>
+      </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" ht="25.5" customHeight="1">
+    <row r="21" spans="1:11" ht="25.5" customHeight="1">
       <c r="A21" s="25">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="27"/>
+      <c r="C21" s="27">
+        <v>4</v>
+      </c>
       <c r="D21" s="28">
         <f>5-C21</f>
-        <v>5</v>
-      </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="29">
+        <v>2</v>
+      </c>
+      <c r="F21" s="32">
+        <v>1</v>
+      </c>
+      <c r="G21" s="33">
+        <v>3</v>
+      </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" ht="25.5" customHeight="1">
+    <row r="22" spans="1:11" ht="25.5" customHeight="1">
       <c r="A22" s="25">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="27"/>
+      <c r="C22" s="27">
+        <v>4</v>
+      </c>
       <c r="D22" s="28">
         <f>C22-1</f>
-        <v>-1</v>
-      </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+        <v>3</v>
+      </c>
+      <c r="E22" s="29">
+        <v>4</v>
+      </c>
+      <c r="F22" s="32">
+        <v>4</v>
+      </c>
+      <c r="G22" s="33">
+        <v>3</v>
+      </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
     </row>
-    <row r="23" ht="25.5" customHeight="1">
+    <row r="23" spans="1:11" ht="25.5" customHeight="1">
       <c r="A23" s="25">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="27"/>
+      <c r="C23" s="27">
+        <v>1</v>
+      </c>
       <c r="D23" s="28">
         <f>5-C23</f>
-        <v>5</v>
-      </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
+        <v>4</v>
+      </c>
+      <c r="E23" s="29">
+        <v>1</v>
+      </c>
+      <c r="F23" s="32">
+        <v>1</v>
+      </c>
+      <c r="G23" s="33">
+        <v>1</v>
+      </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" ht="25.5" customHeight="1">
+    <row r="24" spans="1:11" ht="25.5" customHeight="1">
       <c r="A24" s="18"/>
       <c r="B24" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="35">
-        <f> ((C14-1)+(5-C15)+(C16-1)+(5-C17)+(C18-1)+(5-C19)+(C20-1)+(5-C21)+(C22-1)+(5-C23))*2.5</f>
-        <v>50</v>
+        <f>((C14-1)+(5-C15)+(C16-1)+(5-C17)+(C18-1)+(5-C19)+(C20-1)+(5-C21)+(C22-1)+(5-C23))*2.5</f>
+        <v>70</v>
       </c>
       <c r="D24" s="36">
         <f>(SUM(D14:D23))*2.5</f>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E24" s="37">
-        <f t="shared" ref="E24:G24" si="1"> ((E14-1)+(5-E15)+(E16-1)+(5-E17)+(E18-1)+(5-E19)+(E20-1)+(5-E21)+(E22-1)+(5-E23))*2.5</f>
-        <v>50</v>
+        <f t="shared" ref="E24:G24" si="0">((E14-1)+(5-E15)+(E16-1)+(5-E17)+(E18-1)+(5-E19)+(E20-1)+(5-E21)+(E22-1)+(5-E23))*2.5</f>
+        <v>75</v>
       </c>
       <c r="F24" s="38">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>85</v>
       </c>
       <c r="G24" s="39">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
     </row>
-    <row r="25" ht="25.5" customHeight="1">
+    <row r="25" spans="1:11" ht="25.5" customHeight="1">
       <c r="B25" s="40" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="41"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="B26" s="40" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="41"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="B27" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
       <c r="B28" s="42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1">
       <c r="B29" s="42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1">
       <c r="B30" s="42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="33" spans="2:2" ht="15.75" customHeight="1">
       <c r="B33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="2:2" ht="15.75" customHeight="1">
       <c r="B34" s="43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="35" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="36" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="37" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="38" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="39" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="40" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="41" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="42" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="43" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="44" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="45" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="46" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="47" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="48" spans="2:2" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2050,18 +2587,17 @@
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations>
+  <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 1 and 5" sqref="C14:C23 E14:G23">
-      <formula1>1.0</formula1>
-      <formula2>5.0</formula2>
+      <formula1>1</formula1>
+      <formula2>5</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B34"/>
+    <hyperlink ref="B34" r:id="rId1"/>
   </hyperlinks>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToWidth="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId2"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup fitToWidth="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>